<commit_message>
Arrow color change 12-3
</commit_message>
<xml_diff>
--- a/data_path.xlsx
+++ b/data_path.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crinamalanciuc/Desktop/ENVR 401/shiny_dashboard_app/final_dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/crinamalanciuc/Desktop/ENVR 401/shiny_dashboard_app/final_dashboard/Diagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C8AF5D5-7FA8-B941-9950-F7873BFE257C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89453DD4-7818-154C-9502-E83066214B55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="680" windowWidth="29400" windowHeight="16500" activeTab="1" xr2:uid="{CAD6C5D5-F399-7543-A5E4-14A94DE37046}"/>
   </bookViews>
@@ -929,7 +929,7 @@
   <dimension ref="A1:I35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="117" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="S19" sqref="S19"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1446,7 +1446,7 @@
         <v>35</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F19" s="3">
         <v>0.44750000000000001</v>

</xml_diff>